<commit_message>
Project 3 done! Quantitative value strategy
</commit_message>
<xml_diff>
--- a/momentum strategy.xlsx
+++ b/momentum strategy.xlsx
@@ -52,34 +52,34 @@
     <t>HQM Score</t>
   </si>
   <si>
+    <t>ADBE</t>
+  </si>
+  <si>
     <t>AAL</t>
   </si>
   <si>
+    <t>ALGN</t>
+  </si>
+  <si>
+    <t>AMAT</t>
+  </si>
+  <si>
+    <t>AOS</t>
+  </si>
+  <si>
+    <t>AAPL</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>ALLE</t>
+  </si>
+  <si>
     <t>ALK</t>
-  </si>
-  <si>
-    <t>AAPL</t>
-  </si>
-  <si>
-    <t>ADBE</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>AMAT</t>
-  </si>
-  <si>
-    <t>AMZN</t>
-  </si>
-  <si>
-    <t>AME</t>
-  </si>
-  <si>
-    <t>ALGN</t>
-  </si>
-  <si>
-    <t>AMD</t>
   </si>
   <si>
     <t>Stock Price</t>
@@ -505,37 +505,37 @@
         <v>12</v>
       </c>
       <c r="B2" s="2">
-        <v>18.35</v>
+        <v>532.23</v>
       </c>
       <c r="C2" s="3">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="D2" s="4">
-        <v>0.3014184397163122</v>
+        <v>0.3615851006677071</v>
       </c>
       <c r="E2" s="4">
         <v>0.8297872340425532</v>
       </c>
       <c r="F2" s="4">
-        <v>0.09031491384432577</v>
+        <v>0.5447553259418354</v>
       </c>
       <c r="G2" s="4">
-        <v>0.7021276595744681</v>
+        <v>0.9787234042553191</v>
       </c>
       <c r="H2" s="4">
-        <v>0.4169884169884173</v>
+        <v>0.4050422386483632</v>
       </c>
       <c r="I2" s="4">
-        <v>1</v>
+        <v>0.9787234042553191</v>
       </c>
       <c r="J2" s="4">
-        <v>0.178548490687219</v>
+        <v>0.1723127753303966</v>
       </c>
       <c r="K2" s="4">
-        <v>1</v>
+        <v>0.9574468085106383</v>
       </c>
       <c r="L2" s="4">
-        <v>0.8829787234042553</v>
+        <v>0.9361702127659575</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -543,34 +543,34 @@
         <v>13</v>
       </c>
       <c r="B3" s="2">
-        <v>53.75</v>
+        <v>18.68</v>
       </c>
       <c r="C3" s="3">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="D3" s="4">
-        <v>0.3119355626067855</v>
+        <v>0.3248226950354609</v>
       </c>
       <c r="E3" s="4">
-        <v>0.8723404255319148</v>
+        <v>0.8085106382978724</v>
       </c>
       <c r="F3" s="4">
-        <v>0.08805668016194335</v>
+        <v>0.1099227569815806</v>
       </c>
       <c r="G3" s="4">
         <v>0.6808510638297872</v>
       </c>
       <c r="H3" s="4">
-        <v>0.2682869277961302</v>
+        <v>0.4424710424710425</v>
       </c>
       <c r="I3" s="4">
-        <v>0.9574468085106383</v>
+        <v>1</v>
       </c>
       <c r="J3" s="4">
-        <v>0.104830421377184</v>
+        <v>0.1997430956968529</v>
       </c>
       <c r="K3" s="4">
-        <v>0.9787234042553191</v>
+        <v>1</v>
       </c>
       <c r="L3" s="4">
         <v>0.8723404255319149</v>
@@ -581,37 +581,37 @@
         <v>14</v>
       </c>
       <c r="B4" s="2">
-        <v>190.68</v>
+        <v>360.62</v>
       </c>
       <c r="C4" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D4" s="4">
-        <v>0.3029039972668262</v>
+        <v>0.3889231243259899</v>
       </c>
       <c r="E4" s="4">
-        <v>0.851063829787234</v>
+        <v>0.8936170212765957</v>
       </c>
       <c r="F4" s="4">
-        <v>0.4292781650550934</v>
+        <v>0.5307751082434842</v>
       </c>
       <c r="G4" s="4">
+        <v>0.9574468085106383</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.05645232166398118</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.4468085106382979</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.1845355406648272</v>
+      </c>
+      <c r="K4" s="4">
         <v>0.9787234042553191</v>
       </c>
-      <c r="H4" s="4">
-        <v>0.1517274704034792</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0.851063829787234</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0.05371352785145889</v>
-      </c>
-      <c r="K4" s="4">
-        <v>0.7446808510638298</v>
-      </c>
       <c r="L4" s="4">
-        <v>0.8563829787234043</v>
+        <v>0.8191489361702128</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -619,37 +619,37 @@
         <v>15</v>
       </c>
       <c r="B5" s="2">
-        <v>485.27</v>
+        <v>144.51</v>
       </c>
       <c r="C5" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D5" s="4">
-        <v>0.241449000997723</v>
+        <v>0.592396694214876</v>
       </c>
       <c r="E5" s="4">
-        <v>0.6595744680851063</v>
+        <v>0.9787234042553191</v>
       </c>
       <c r="F5" s="4">
-        <v>0.4084576536831717</v>
+        <v>0.3113430127041741</v>
       </c>
       <c r="G5" s="4">
-        <v>0.9574468085106383</v>
+        <v>0.851063829787234</v>
       </c>
       <c r="H5" s="4">
-        <v>0.2810718057022175</v>
+        <v>0.2735524808319378</v>
       </c>
       <c r="I5" s="4">
-        <v>0.9787234042553191</v>
+        <v>0.9148936170212765</v>
       </c>
       <c r="J5" s="4">
-        <v>0.06887665198237891</v>
+        <v>0.06163679106670572</v>
       </c>
       <c r="K5" s="4">
-        <v>0.8085106382978724</v>
+        <v>0.4468085106382979</v>
       </c>
       <c r="L5" s="4">
-        <v>0.851063829787234</v>
+        <v>0.7978723404255319</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -657,37 +657,37 @@
         <v>16</v>
       </c>
       <c r="B6" s="2">
-        <v>190.86</v>
+        <v>76.51000000000001</v>
       </c>
       <c r="C6" s="3">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D6" s="4">
-        <v>0.3556360536969958</v>
+        <v>0.2835094782754572</v>
       </c>
       <c r="E6" s="4">
-        <v>0.8936170212765957</v>
+        <v>0.6595744680851063</v>
       </c>
       <c r="F6" s="4">
-        <v>0.1574287446937539</v>
+        <v>0.2460912052117266</v>
       </c>
       <c r="G6" s="4">
         <v>0.8297872340425532</v>
       </c>
       <c r="H6" s="4">
-        <v>0.1402796032978852</v>
+        <v>0.153127354935946</v>
       </c>
       <c r="I6" s="4">
         <v>0.8085106382978724</v>
       </c>
       <c r="J6" s="4">
-        <v>0.07092357760071821</v>
+        <v>0.1122256141881086</v>
       </c>
       <c r="K6" s="4">
-        <v>0.851063829787234</v>
+        <v>0.8297872340425532</v>
       </c>
       <c r="L6" s="4">
-        <v>0.8457446808510638</v>
+        <v>0.7819148936170213</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -695,37 +695,37 @@
         <v>17</v>
       </c>
       <c r="B7" s="2">
-        <v>139.57</v>
+        <v>193.73</v>
       </c>
       <c r="C7" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" s="4">
-        <v>0.5379614325068869</v>
+        <v>0.3237444482405192</v>
       </c>
       <c r="E7" s="4">
-        <v>0.9787234042553191</v>
+        <v>0.7872340425531915</v>
       </c>
       <c r="F7" s="4">
-        <v>0.2665154264972776</v>
+        <v>0.4521400194887939</v>
       </c>
       <c r="G7" s="4">
+        <v>0.9148936170212765</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.1701497946363855</v>
+      </c>
+      <c r="I7" s="4">
         <v>0.851063829787234</v>
       </c>
-      <c r="H7" s="4">
-        <v>0.2300167445139685</v>
-      </c>
-      <c r="I7" s="4">
-        <v>0.9148936170212765</v>
-      </c>
       <c r="J7" s="4">
-        <v>0.02534528357331767</v>
+        <v>0.07056808134394332</v>
       </c>
       <c r="K7" s="4">
-        <v>0.4893617021276596</v>
+        <v>0.5319148936170213</v>
       </c>
       <c r="L7" s="4">
-        <v>0.8085106382978723</v>
+        <v>0.7712765957446808</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -733,37 +733,37 @@
         <v>18</v>
       </c>
       <c r="B8" s="2">
-        <v>129.78</v>
+        <v>192.39</v>
       </c>
       <c r="C8" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8" s="4">
-        <v>0.1156193587208802</v>
+        <v>0.3665033027913913</v>
       </c>
       <c r="E8" s="4">
-        <v>0.4893617021276596</v>
+        <v>0.851063829787234</v>
       </c>
       <c r="F8" s="4">
-        <v>0.3622336517266715</v>
+        <v>0.1667070952092176</v>
       </c>
       <c r="G8" s="4">
-        <v>0.9148936170212765</v>
+        <v>0.7872340425531915</v>
       </c>
       <c r="H8" s="4">
-        <v>0.2673828125</v>
+        <v>0.149420480344127</v>
       </c>
       <c r="I8" s="4">
-        <v>0.9361702127659575</v>
+        <v>0.7659574468085105</v>
       </c>
       <c r="J8" s="4">
-        <v>0.0514461638175483</v>
+        <v>0.07950847267422279</v>
       </c>
       <c r="K8" s="4">
-        <v>0.7234042553191489</v>
+        <v>0.6808510638297872</v>
       </c>
       <c r="L8" s="4">
-        <v>0.7659574468085106</v>
+        <v>0.7712765957446808</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -771,37 +771,37 @@
         <v>19</v>
       </c>
       <c r="B9" s="2">
-        <v>157.08</v>
+        <v>352.46</v>
       </c>
       <c r="C9" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D9" s="4">
-        <v>0.3850630455868091</v>
+        <v>0.4792462332647835</v>
       </c>
       <c r="E9" s="4">
-        <v>0.9148936170212765</v>
+        <v>0.9361702127659575</v>
       </c>
       <c r="F9" s="4">
-        <v>0.07921676399862587</v>
+        <v>0.06428722408430709</v>
       </c>
       <c r="G9" s="4">
-        <v>0.6595744680851063</v>
+        <v>0.5319148936170213</v>
       </c>
       <c r="H9" s="4">
-        <v>0.1345612134344532</v>
+        <v>0.1430146581917238</v>
       </c>
       <c r="I9" s="4">
-        <v>0.7872340425531915</v>
+        <v>0.7234042553191489</v>
       </c>
       <c r="J9" s="4">
-        <v>0.04517931998136948</v>
+        <v>0.1212342929855255</v>
       </c>
       <c r="K9" s="4">
-        <v>0.6595744680851063</v>
+        <v>0.8936170212765957</v>
       </c>
       <c r="L9" s="4">
-        <v>0.7553191489361701</v>
+        <v>0.7712765957446808</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -809,37 +809,37 @@
         <v>20</v>
       </c>
       <c r="B10" s="2">
-        <v>329.54</v>
+        <v>125.6</v>
       </c>
       <c r="C10" s="3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D10" s="4">
-        <v>0.2692189185025422</v>
+        <v>0.2434412434412434</v>
       </c>
       <c r="E10" s="4">
-        <v>0.7659574468085105</v>
+        <v>0.5957446808510638</v>
       </c>
       <c r="F10" s="4">
-        <v>0.3988454028355548</v>
+        <v>0.106510439608845</v>
       </c>
       <c r="G10" s="4">
-        <v>0.9361702127659575</v>
+        <v>0.6595744680851063</v>
       </c>
       <c r="H10" s="4">
-        <v>-0.03459792002343631</v>
+        <v>0.2296847464264733</v>
       </c>
       <c r="I10" s="4">
-        <v>0.3191489361702128</v>
+        <v>0.8723404255319148</v>
       </c>
       <c r="J10" s="4">
-        <v>0.08244645907239523</v>
+        <v>0.1149578339991122</v>
       </c>
       <c r="K10" s="4">
-        <v>0.9148936170212765</v>
+        <v>0.8723404255319148</v>
       </c>
       <c r="L10" s="4">
-        <v>0.7340425531914894</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -847,37 +847,37 @@
         <v>21</v>
       </c>
       <c r="B11" s="2">
-        <v>113.17</v>
+        <v>53.42</v>
       </c>
       <c r="C11" s="3">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D11" s="4">
-        <v>0.4271122320302649</v>
+        <v>0.3038808884549671</v>
       </c>
       <c r="E11" s="4">
-        <v>0.9574468085106383</v>
+        <v>0.7446808510638298</v>
       </c>
       <c r="F11" s="4">
-        <v>0.5984463276836158</v>
+        <v>0.08137651821862346</v>
       </c>
       <c r="G11" s="4">
-        <v>1</v>
+        <v>0.574468085106383</v>
       </c>
       <c r="H11" s="4">
-        <v>0.2289065045064611</v>
+        <v>0.2605002359603585</v>
       </c>
       <c r="I11" s="4">
         <v>0.8936170212765957</v>
       </c>
       <c r="J11" s="4">
-        <v>-0.09406019852705727</v>
+        <v>0.09804727646454281</v>
       </c>
       <c r="K11" s="4">
-        <v>0.02127659574468085</v>
+        <v>0.7872340425531915</v>
       </c>
       <c r="L11" s="4">
-        <v>0.7180851063829787</v>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>